<commit_message>
tweaks and updates to importer and flow
</commit_message>
<xml_diff>
--- a/public/Diffusion Marketplace.xlsx
+++ b/public/Diffusion Marketplace.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="442">
   <si>
     <t>Respondent ID</t>
   </si>
@@ -1000,6 +1000,9 @@
     <t>We need this information. I think it is another 10-20 that are implementing the practice now. We need the contacts.</t>
   </si>
   <si>
+    <t>pills_1000x550-730x402.png</t>
+  </si>
+  <si>
     <t>3 months</t>
   </si>
   <si>
@@ -1012,7 +1015,7 @@
     <t>Deprescribing medications using this approach has resulted in decreased pill burden and improved utilization of human and economic resources. At Central Arkansas VA Medical Center, between February 2016 and September 2018, over 8,400 Veterans have benefited from the program with almost 15,000 prescriptions deprescribed.  Eight other VA facilities have implemented VIONE. More than 18,000 medications have been discontinued in over 10,000 Veterans and the VIONE tool was exported to 31 VA medical centers.  VIONE has improved patient safety and increased patient quality of life.</t>
   </si>
   <si>
-    <t>$$$$ - Greater than $1M in cost avoidance.</t>
+    <t>4. $$$$ - Greater than $1M in cost avoidance.</t>
   </si>
   <si>
     <t>4. High or large Human Impact</t>
@@ -1081,12 +1084,6 @@
     <t>Air Force Veteran Barry Mitchell Vuletich tells Dr. Battar, “The lesser medicines I have to take, the better off I am.”</t>
   </si>
   <si>
-    <t>Dr. Battar/MD</t>
-  </si>
-  <si>
-    <t>same list as the first few questions/5 total</t>
-  </si>
-  <si>
     <t>I'm not sure how to steal photos from web sites or news articles that the VA has already published. Is that a legitimate source of quotes/photos/etc.? Can we just republish and list the source.   https://www.blogs.va.gov/VAntage/53716/helping-veterans-stop-unnecessary-medications/</t>
   </si>
   <si>
@@ -1120,7 +1117,7 @@
     <t xml:space="preserve">Puget Sound Health Care System </t>
   </si>
   <si>
-    <t>Complexity Level 1a Largest levels of volume, patient risk, teaching and research Largest number and breadth of physician specialists. Level 1a facilities contain level 5 Intensive Care Unit (ICU) units.</t>
+    <t>(1a) Complexity Level 1a Largest levels of volume, patient risk, teaching and research Largest number and breadth of physician specialists. Level 1a facilities contain level 5 Intensive Care Unit (ICU) units.</t>
   </si>
   <si>
     <t>Prosthetics and Rehabilitation</t>
@@ -1183,7 +1180,7 @@
     <t>FLOW3 is a system of three interrelated software platforms that automate, standardize, and provide transparency into the limb acquisition process. FLOW3 begins in-clinic with physician entry of a prosthesis prescription using the FLOW Consult Templates. The order then moves to the prosthetist, who enters the appropriate codes using the Consult Comment Tool. Then, purchasing agents use the Web-based App to generate the quote for force entry, which contracting staff can access the very next day.</t>
   </si>
   <si>
-    <t>$$ - Between $10,000 and $100,000 in annual cost avoidance</t>
+    <t>2. $$ - Between $10,000 and $100,000 in annual cost avoidance</t>
   </si>
   <si>
     <t>If FLOW3 champions do not allocate sufficient time to training their site the implementation process will be slow and time savings will not be achieved.</t>
@@ -1231,16 +1228,16 @@
     <t>Dr. Jeffrey Heckman, a physician in the VA Puget Sound Health Care System, treated many Veterans frustrated by the lengthy process of receiving their prosthetic limbs. Motivated by one such Veteran, who offered his own technical services to improve the process, Dr. Heckman gathered a team, consisting of prosthetist Wayne Biggs and data system expert Jeffrey Bott, to overhaul and automate the prosthetic limb acquisition process. The result was a system of three interrelated software platforms, known as FLOW3, that streamlines and provides transparency into the acquisition flow. After successful implementation at Puget Sound, the team spread their innovation through the Diffusion of Excellence program, beginning with a partnership with Dawn Schwarten at the Milwaukee VA Medical Center and ultimately rolling FLOW3 out across VISN 12.</t>
   </si>
   <si>
-    <t>Dr. Jeffrey T. Heckman/Clinical Lead and Gold Status Fellow</t>
-  </si>
-  <si>
-    <t>Jeff Bott/Technical Lead</t>
-  </si>
-  <si>
-    <t>Wayne Biggs/Coding and Template Lead</t>
-  </si>
-  <si>
-    <t>Brian Stevenson/Diffusion Specialist</t>
+    <t>Dr. Jeffrey T. Heckman\Clinical Lead and Gold Status Fellow</t>
+  </si>
+  <si>
+    <t>Jeff Bott\Technical Lead</t>
+  </si>
+  <si>
+    <t>Wayne Biggs\Coding and Template Lead</t>
+  </si>
+  <si>
+    <t>Brian Stevenson\Diffusion Specialist</t>
   </si>
   <si>
     <t>heckman_jeff.jpg</t>
@@ -1309,7 +1306,7 @@
     <t>This practice ensures inpatient, non-ventilator Veterans receive oral care by providing consistent staff training, educating patients on oral care and its association with pneumonia, and standardizing the procurement process for obtaining oral care supplies. HAPPEN is low cost to implement (less than $5.00 per patient for oral care supplies), has a high return on investment, and enhances the quality of care provided to Veterans. Nurses. By engaging Veterans in proper oral care practices, nurses can teach Veterans about the importance of good oral hygiene, and its ability to reduce Veterans’ hospital stays, while reducing the risk of readmission.</t>
   </si>
   <si>
-    <t>$$$ - Between $100,000 and $1 Million</t>
+    <t>3. $$$ - Between $100,000 and $1 Million</t>
   </si>
   <si>
     <t>Non reporting and inconsistencies in reporting can make it hard to tell if the practice is being used correctly</t>
@@ -4225,7 +4222,7 @@
         <v>43520.39091435185</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>43520.42805555555</v>
+        <v>43525.04221064815</v>
       </c>
       <c r="E6" t="s">
         <v>307</v>
@@ -4560,7 +4557,9 @@
       <c r="HM6" t="s">
         <v>327</v>
       </c>
-      <c r="HN6" t="s"/>
+      <c r="HN6" t="s">
+        <v>328</v>
+      </c>
       <c r="HO6" t="s"/>
       <c r="HP6" t="s"/>
       <c r="HQ6" t="s"/>
@@ -4590,54 +4589,54 @@
       <c r="IK6" t="s"/>
       <c r="IL6" t="s"/>
       <c r="IM6" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="IN6" t="s"/>
       <c r="IO6" t="s"/>
       <c r="IP6" t="s"/>
       <c r="IQ6" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="IR6" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="IS6" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="IT6" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="IU6" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="IV6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="IW6" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="IX6" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="IY6" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="IZ6" t="s"/>
       <c r="JA6" t="s"/>
       <c r="JB6" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="JC6" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="JD6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="JE6" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="JF6" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="JG6" t="s">
         <v>220</v>
@@ -4664,61 +4663,61 @@
       <c r="JS6" t="s"/>
       <c r="JT6" t="s"/>
       <c r="JU6" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="JV6" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="JW6" t="s"/>
       <c r="JX6" t="s"/>
       <c r="JY6" t="s"/>
       <c r="JZ6" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="KA6" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="KB6" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="KC6" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="KD6" t="s"/>
       <c r="KE6" t="s"/>
       <c r="KF6" t="s"/>
       <c r="KG6" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="KH6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="KI6" t="s"/>
       <c r="KJ6" t="s"/>
       <c r="KK6" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="KL6" t="s"/>
       <c r="KM6" t="s"/>
       <c r="KN6" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="KO6" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="KP6" t="s"/>
       <c r="KQ6" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="KR6" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="KS6" t="s"/>
       <c r="KT6" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="KU6" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="KV6" t="s"/>
       <c r="KW6" t="s"/>
@@ -4727,21 +4726,25 @@
       <c r="KZ6" t="s"/>
       <c r="LA6" t="s"/>
       <c r="LB6" t="s">
-        <v>355</v>
-      </c>
-      <c r="LC6" t="s">
-        <v>356</v>
-      </c>
-      <c r="LD6" t="s"/>
-      <c r="LE6" t="s"/>
-      <c r="LF6" t="s"/>
+        <v>310</v>
+      </c>
+      <c r="LC6" t="s"/>
+      <c r="LD6" t="s">
+        <v>311</v>
+      </c>
+      <c r="LE6" t="s">
+        <v>312</v>
+      </c>
+      <c r="LF6" t="s">
+        <v>313</v>
+      </c>
       <c r="LG6" t="s"/>
       <c r="LH6" t="s"/>
       <c r="LI6" t="s"/>
       <c r="LJ6" t="s"/>
       <c r="LK6" t="s"/>
       <c r="LL6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7" spans="1:324">
@@ -4755,22 +4758,22 @@
         <v>43518.48881944444</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>43524.4716087963</v>
+        <v>43525.04128472223</v>
       </c>
       <c r="E7" t="s">
+        <v>357</v>
+      </c>
+      <c r="F7" t="s">
         <v>358</v>
-      </c>
-      <c r="F7" t="s">
-        <v>359</v>
       </c>
       <c r="G7" t="s"/>
       <c r="H7" t="s"/>
       <c r="I7" t="s"/>
       <c r="J7" t="s">
+        <v>359</v>
+      </c>
+      <c r="K7" t="s">
         <v>360</v>
-      </c>
-      <c r="K7" t="s">
-        <v>361</v>
       </c>
       <c r="L7" t="s"/>
       <c r="M7" t="s">
@@ -4784,21 +4787,21 @@
       <c r="S7" t="s"/>
       <c r="T7" t="s"/>
       <c r="U7" t="s">
+        <v>361</v>
+      </c>
+      <c r="V7" t="s">
         <v>362</v>
       </c>
-      <c r="V7" t="s">
+      <c r="W7" t="s">
         <v>363</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>364</v>
-      </c>
-      <c r="X7" t="s">
-        <v>365</v>
       </c>
       <c r="Y7" t="s"/>
       <c r="Z7" t="s"/>
       <c r="AA7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AB7" t="s"/>
       <c r="AC7" t="s">
@@ -4832,10 +4835,10 @@
       <c r="AY7" t="s"/>
       <c r="AZ7" t="s"/>
       <c r="BA7" t="s">
+        <v>366</v>
+      </c>
+      <c r="BB7" t="s">
         <v>367</v>
-      </c>
-      <c r="BB7" t="s">
-        <v>368</v>
       </c>
       <c r="BC7" t="s"/>
       <c r="BD7" t="s">
@@ -4903,7 +4906,7 @@
       <c r="CT7" t="s"/>
       <c r="CU7" t="s"/>
       <c r="CV7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="CW7" t="s"/>
       <c r="CX7" t="s"/>
@@ -4929,16 +4932,16 @@
       <c r="DP7" t="s"/>
       <c r="DQ7" t="s"/>
       <c r="DR7" t="s">
+        <v>369</v>
+      </c>
+      <c r="DS7" t="s">
         <v>370</v>
       </c>
-      <c r="DS7" t="s">
+      <c r="DT7" t="s">
         <v>371</v>
       </c>
-      <c r="DT7" t="s">
+      <c r="DU7" t="s">
         <v>372</v>
-      </c>
-      <c r="DU7" t="s">
-        <v>373</v>
       </c>
       <c r="DV7" t="s"/>
       <c r="DW7" t="s">
@@ -4983,7 +4986,7 @@
       <c r="EV7" t="s"/>
       <c r="EW7" t="s"/>
       <c r="EX7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="EY7" t="s"/>
       <c r="EZ7" t="s"/>
@@ -5070,28 +5073,28 @@
       <c r="HE7" t="s"/>
       <c r="HF7" t="s"/>
       <c r="HG7" t="s">
+        <v>374</v>
+      </c>
+      <c r="HH7" t="s">
         <v>375</v>
       </c>
-      <c r="HH7" t="s">
+      <c r="HI7" t="s">
         <v>376</v>
       </c>
-      <c r="HI7" t="s">
+      <c r="HJ7" t="s">
         <v>377</v>
-      </c>
-      <c r="HJ7" t="s">
-        <v>378</v>
       </c>
       <c r="HK7" t="n">
         <v>2</v>
       </c>
       <c r="HL7" t="s">
+        <v>378</v>
+      </c>
+      <c r="HM7" t="s">
         <v>379</v>
       </c>
-      <c r="HM7" t="s">
+      <c r="HN7" t="s">
         <v>380</v>
-      </c>
-      <c r="HN7" t="s">
-        <v>381</v>
       </c>
       <c r="HO7" t="s"/>
       <c r="HP7" t="s"/>
@@ -5101,13 +5104,13 @@
       <c r="HT7" t="s"/>
       <c r="HU7" t="s"/>
       <c r="HV7" t="s">
+        <v>381</v>
+      </c>
+      <c r="HW7" t="s">
         <v>382</v>
       </c>
-      <c r="HW7" t="s">
+      <c r="HX7" t="s">
         <v>383</v>
-      </c>
-      <c r="HX7" t="s">
-        <v>384</v>
       </c>
       <c r="HY7" t="s"/>
       <c r="HZ7" t="s"/>
@@ -5129,50 +5132,50 @@
       </c>
       <c r="IK7" t="s"/>
       <c r="IL7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="IM7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="IN7" t="s"/>
       <c r="IO7" t="s"/>
       <c r="IP7" t="s"/>
       <c r="IQ7" t="s">
+        <v>385</v>
+      </c>
+      <c r="IR7" t="s">
         <v>386</v>
       </c>
-      <c r="IR7" t="s">
+      <c r="IS7" t="s">
         <v>387</v>
       </c>
-      <c r="IS7" t="s">
+      <c r="IT7" t="s">
         <v>388</v>
       </c>
-      <c r="IT7" t="s">
+      <c r="IU7" t="s">
+        <v>334</v>
+      </c>
+      <c r="IV7" t="s">
         <v>389</v>
       </c>
-      <c r="IU7" t="s">
-        <v>333</v>
-      </c>
-      <c r="IV7" t="s">
+      <c r="IW7" t="s">
         <v>390</v>
-      </c>
-      <c r="IW7" t="s">
-        <v>391</v>
       </c>
       <c r="IX7" t="s"/>
       <c r="IY7" t="s"/>
       <c r="IZ7" t="s"/>
       <c r="JA7" t="s"/>
       <c r="JB7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="JC7" t="s">
+        <v>391</v>
+      </c>
+      <c r="JD7" t="s">
         <v>392</v>
       </c>
-      <c r="JD7" t="s">
-        <v>393</v>
-      </c>
       <c r="JE7" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="JF7" t="s"/>
       <c r="JG7" t="s"/>
@@ -5195,51 +5198,51 @@
       <c r="JX7" t="s"/>
       <c r="JY7" t="s"/>
       <c r="JZ7" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="KA7" t="s">
+        <v>393</v>
+      </c>
+      <c r="KB7" t="s">
         <v>394</v>
       </c>
-      <c r="KB7" t="s">
+      <c r="KC7" t="s">
         <v>395</v>
       </c>
-      <c r="KC7" t="s">
+      <c r="KD7" t="s">
         <v>396</v>
       </c>
-      <c r="KD7" t="s">
+      <c r="KE7" t="s">
         <v>397</v>
-      </c>
-      <c r="KE7" t="s">
-        <v>398</v>
       </c>
       <c r="KF7" t="s"/>
       <c r="KG7" t="s"/>
       <c r="KH7" t="s">
+        <v>398</v>
+      </c>
+      <c r="KI7" t="s">
         <v>399</v>
-      </c>
-      <c r="KI7" t="s">
-        <v>400</v>
       </c>
       <c r="KJ7" t="s"/>
       <c r="KK7" t="s">
+        <v>400</v>
+      </c>
+      <c r="KL7" t="s">
         <v>401</v>
-      </c>
-      <c r="KL7" t="s">
-        <v>402</v>
       </c>
       <c r="KM7" t="s"/>
       <c r="KN7" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="KO7" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="KP7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="KQ7" t="s"/>
       <c r="KR7" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="KS7" t="s"/>
       <c r="KT7" t="s"/>
@@ -5251,29 +5254,29 @@
       <c r="KZ7" t="s"/>
       <c r="LA7" t="s"/>
       <c r="LB7" t="s">
+        <v>404</v>
+      </c>
+      <c r="LC7" t="s">
         <v>405</v>
       </c>
-      <c r="LC7" t="s">
+      <c r="LD7" t="s">
         <v>406</v>
       </c>
-      <c r="LD7" t="s">
+      <c r="LE7" t="s">
         <v>407</v>
-      </c>
-      <c r="LE7" t="s">
-        <v>408</v>
       </c>
       <c r="LF7" t="s"/>
       <c r="LG7" t="s">
+        <v>408</v>
+      </c>
+      <c r="LH7" t="s">
         <v>409</v>
       </c>
-      <c r="LH7" t="s">
+      <c r="LI7" t="s">
         <v>410</v>
       </c>
-      <c r="LI7" t="s">
+      <c r="LJ7" t="s">
         <v>411</v>
-      </c>
-      <c r="LJ7" t="s">
-        <v>412</v>
       </c>
       <c r="LK7" t="s"/>
       <c r="LL7" t="s"/>
@@ -5292,19 +5295,19 @@
         <v>43518.56435185186</v>
       </c>
       <c r="E8" t="s">
+        <v>412</v>
+      </c>
+      <c r="F8" t="s">
         <v>413</v>
-      </c>
-      <c r="F8" t="s">
-        <v>414</v>
       </c>
       <c r="G8" t="s"/>
       <c r="H8" t="s"/>
       <c r="I8" t="s"/>
       <c r="J8" t="s">
+        <v>414</v>
+      </c>
+      <c r="K8" t="s">
         <v>415</v>
-      </c>
-      <c r="K8" t="s">
-        <v>416</v>
       </c>
       <c r="L8" t="s"/>
       <c r="M8" t="s"/>
@@ -5316,21 +5319,21 @@
       <c r="S8" t="s"/>
       <c r="T8" t="s"/>
       <c r="U8" t="s">
+        <v>416</v>
+      </c>
+      <c r="V8" t="s">
         <v>417</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>418</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>419</v>
-      </c>
-      <c r="X8" t="s">
-        <v>420</v>
       </c>
       <c r="Y8" t="s"/>
       <c r="Z8" t="s"/>
       <c r="AA8" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AB8" t="s"/>
       <c r="AC8" t="s">
@@ -5362,7 +5365,7 @@
       <c r="AY8" t="s"/>
       <c r="AZ8" t="s"/>
       <c r="BA8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="BB8" t="s"/>
       <c r="BC8" t="s"/>
@@ -5441,13 +5444,13 @@
       <c r="DP8" t="s"/>
       <c r="DQ8" t="s"/>
       <c r="DR8" t="s">
+        <v>422</v>
+      </c>
+      <c r="DS8" t="s">
         <v>423</v>
       </c>
-      <c r="DS8" t="s">
+      <c r="DT8" t="s">
         <v>424</v>
-      </c>
-      <c r="DT8" t="s">
-        <v>425</v>
       </c>
       <c r="DU8" t="s"/>
       <c r="DV8" t="s"/>
@@ -5569,11 +5572,11 @@
       <c r="HT8" t="s"/>
       <c r="HU8" t="s"/>
       <c r="HV8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="HW8" t="s"/>
       <c r="HX8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="HY8" t="s"/>
       <c r="HZ8" t="s"/>
@@ -5591,54 +5594,54 @@
       </c>
       <c r="IK8" t="s"/>
       <c r="IL8" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="IM8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="IN8" t="s"/>
       <c r="IO8" t="s"/>
       <c r="IP8" t="s"/>
       <c r="IQ8" t="s">
+        <v>427</v>
+      </c>
+      <c r="IR8" t="s">
         <v>428</v>
       </c>
-      <c r="IR8" t="s">
+      <c r="IS8" t="s">
         <v>429</v>
       </c>
-      <c r="IS8" t="s">
+      <c r="IT8" t="s">
         <v>430</v>
       </c>
-      <c r="IT8" t="s">
+      <c r="IU8" t="s">
+        <v>334</v>
+      </c>
+      <c r="IV8" t="s">
         <v>431</v>
       </c>
-      <c r="IU8" t="s">
-        <v>333</v>
-      </c>
-      <c r="IV8" t="s">
+      <c r="IW8" t="s">
         <v>432</v>
       </c>
-      <c r="IW8" t="s">
+      <c r="IX8" t="s">
         <v>433</v>
       </c>
-      <c r="IX8" t="s">
+      <c r="IY8" t="s">
         <v>434</v>
-      </c>
-      <c r="IY8" t="s">
-        <v>435</v>
       </c>
       <c r="IZ8" t="s"/>
       <c r="JA8" t="s"/>
       <c r="JB8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="JC8" t="s">
+        <v>391</v>
+      </c>
+      <c r="JD8" t="s">
         <v>392</v>
       </c>
-      <c r="JD8" t="s">
-        <v>393</v>
-      </c>
       <c r="JE8" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="JF8" t="s"/>
       <c r="JG8" t="s"/>
@@ -5661,7 +5664,7 @@
       <c r="JX8" t="s"/>
       <c r="JY8" t="s"/>
       <c r="JZ8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="KA8" t="s"/>
       <c r="KB8" t="s"/>
@@ -5670,33 +5673,33 @@
       <c r="KE8" t="s"/>
       <c r="KF8" t="s"/>
       <c r="KG8" t="s">
+        <v>435</v>
+      </c>
+      <c r="KH8" t="s">
         <v>436</v>
-      </c>
-      <c r="KH8" t="s">
-        <v>437</v>
       </c>
       <c r="KI8" t="s"/>
       <c r="KJ8" t="s"/>
       <c r="KK8" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="KL8" t="s"/>
       <c r="KM8" t="s"/>
       <c r="KN8" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="KO8" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="KP8" t="s"/>
       <c r="KQ8" t="s"/>
       <c r="KR8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="KS8" t="s"/>
       <c r="KT8" t="s"/>
       <c r="KU8" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="KV8" t="s"/>
       <c r="KW8" t="s"/>
@@ -5705,7 +5708,7 @@
       <c r="KZ8" t="s"/>
       <c r="LA8" t="s"/>
       <c r="LB8" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="LC8" t="s"/>
       <c r="LD8" t="s"/>
@@ -5735,7 +5738,7 @@
         <v>307</v>
       </c>
       <c r="F9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G9" t="s"/>
       <c r="H9" t="s"/>

</xml_diff>